<commit_message>
This commit adds staging, view, and population sql scripts as well as changes made to mapping.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Product.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3416213D-8CA5-4346-AB06-E0DFC02FED2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7129A107-8840-42A4-A39D-6E041605D437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -633,20 +633,20 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -658,7 +658,7 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -694,7 +694,7 @@
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="E4" s="18"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
@@ -730,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="6" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -766,7 +766,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -786,7 +786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
@@ -806,7 +806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
@@ -842,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -862,7 +862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -898,7 +898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
@@ -918,7 +918,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -938,7 +938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>5</v>
       </c>
@@ -958,7 +958,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -978,7 +978,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>5</v>
       </c>
@@ -998,7 +998,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Adding SQL and SLN files
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Product.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7129A107-8840-42A4-A39D-6E041605D437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA42668-3A05-4B87-9F34-3377CEA4868E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>